<commit_message>
Ajout du lien HLK-5M05
</commit_message>
<xml_diff>
--- a/EasyEDA/MAGIC-HOOVER-TRANS/BOM_MAGIC-HOOVER-TRANS_2025-06-01.xlsx
+++ b/EasyEDA/MAGIC-HOOVER-TRANS/BOM_MAGIC-HOOVER-TRANS_2025-06-01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>https://s.click.aliexpress.com/e/_oFlFyPw</t>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_onkmoao</t>
   </si>
 </sst>
 </file>
@@ -1238,7 +1241,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,6 +1766,9 @@
       </c>
       <c r="O11" s="3" t="s">
         <v>80</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2042,11 +2048,12 @@
     <hyperlink ref="P16" r:id="rId24"/>
     <hyperlink ref="P17" r:id="rId25"/>
     <hyperlink ref="P14" r:id="rId26"/>
+    <hyperlink ref="P11" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId28"/>
   <tableParts count="1">
-    <tablePart r:id="rId28"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>